<commit_message>
Moving towards team search functionality
</commit_message>
<xml_diff>
--- a/backend/csv/churnQuery.xlsx
+++ b/backend/csv/churnQuery.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="124">
   <si>
     <t>reason</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>Ming-Chen Hsu</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
   <si>
     <t>[SP:11022-SP12] AggresiveUss SCs Fix</t>
@@ -1196,25 +1202,25 @@
         <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="J6" t="s">
         <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N6" t="s">
         <v>41</v>
@@ -1270,10 +1276,10 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -1285,25 +1291,25 @@
         <v>64</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
         <v>38</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N7" t="s">
         <v>41</v>
@@ -1359,10 +1365,10 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
@@ -1374,28 +1380,28 @@
         <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="J8" t="s">
         <v>38</v>
       </c>
       <c r="K8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="O8">
         <v>4</v>
@@ -1494,25 +1500,25 @@
         <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1544,13 +1550,13 @@
         <v>40</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M2">
         <v>38</v>
@@ -1594,13 +1600,13 @@
         <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M3">
         <v>2</v>
@@ -1644,13 +1650,13 @@
         <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M4">
         <v>2</v>
@@ -1694,13 +1700,13 @@
         <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M5">
         <v>5</v>
@@ -1744,13 +1750,13 @@
         <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M6">
         <v>77</v>
@@ -1794,13 +1800,13 @@
         <v>40</v>
       </c>
       <c r="J7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M7">
         <v>25</v>
@@ -1844,13 +1850,13 @@
         <v>40</v>
       </c>
       <c r="J8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M8">
         <v>2</v>
@@ -1894,13 +1900,13 @@
         <v>40</v>
       </c>
       <c r="J9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M9">
         <v>5</v>
@@ -1944,13 +1950,13 @@
         <v>40</v>
       </c>
       <c r="J10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M10">
         <v>171</v>
@@ -1994,13 +2000,13 @@
         <v>47</v>
       </c>
       <c r="J11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M11">
         <v>6</v>
@@ -2044,13 +2050,13 @@
         <v>47</v>
       </c>
       <c r="J12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M12">
         <v>10</v>
@@ -2094,13 +2100,13 @@
         <v>47</v>
       </c>
       <c r="J13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -2144,13 +2150,13 @@
         <v>47</v>
       </c>
       <c r="J14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M14">
         <v>348</v>
@@ -2194,13 +2200,13 @@
         <v>54</v>
       </c>
       <c r="J15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L15" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -2244,13 +2250,13 @@
         <v>54</v>
       </c>
       <c r="J16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L16" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -2294,13 +2300,13 @@
         <v>54</v>
       </c>
       <c r="J17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K17" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -2344,13 +2350,13 @@
         <v>54</v>
       </c>
       <c r="J18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="L18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M18">
         <v>4</v>
@@ -2394,13 +2400,13 @@
         <v>54</v>
       </c>
       <c r="J19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="L19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M19">
         <v>189</v>
@@ -2444,13 +2450,13 @@
         <v>54</v>
       </c>
       <c r="J20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K20" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L20" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -2494,13 +2500,13 @@
         <v>54</v>
       </c>
       <c r="J21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K21" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L21" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M21">
         <v>3</v>
@@ -2544,13 +2550,13 @@
         <v>54</v>
       </c>
       <c r="J22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K22" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L22" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -2594,13 +2600,13 @@
         <v>54</v>
       </c>
       <c r="J23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="L23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M23">
         <v>3</v>
@@ -2644,13 +2650,13 @@
         <v>54</v>
       </c>
       <c r="J24" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K24" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L24" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M24">
         <v>38</v>
@@ -2694,13 +2700,13 @@
         <v>54</v>
       </c>
       <c r="J25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M25">
         <v>328</v>
@@ -2744,13 +2750,13 @@
         <v>54</v>
       </c>
       <c r="J26" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K26" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L26" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M26">
         <v>40</v>
@@ -2794,13 +2800,13 @@
         <v>54</v>
       </c>
       <c r="J27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K27" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M27">
         <v>253</v>
@@ -2844,13 +2850,13 @@
         <v>54</v>
       </c>
       <c r="J28" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K28" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L28" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M28">
         <v>2</v>
@@ -2894,13 +2900,13 @@
         <v>54</v>
       </c>
       <c r="J29" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K29" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L29" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M29">
         <v>4</v>
@@ -2944,13 +2950,13 @@
         <v>54</v>
       </c>
       <c r="J30" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K30" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L30" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M30">
         <v>4</v>
@@ -2994,13 +3000,13 @@
         <v>54</v>
       </c>
       <c r="J31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K31" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="L31" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M31">
         <v>269</v>
@@ -3044,13 +3050,13 @@
         <v>60</v>
       </c>
       <c r="J32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L32" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M32">
         <v>5</v>
@@ -3094,13 +3100,13 @@
         <v>60</v>
       </c>
       <c r="J33" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K33" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L33" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M33">
         <v>8</v>
@@ -3144,13 +3150,13 @@
         <v>60</v>
       </c>
       <c r="J34" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L34" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M34">
         <v>11</v>
@@ -3194,13 +3200,13 @@
         <v>60</v>
       </c>
       <c r="J35" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K35" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L35" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M35">
         <v>6</v>
@@ -3244,13 +3250,13 @@
         <v>60</v>
       </c>
       <c r="J36" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K36" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L36" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M36">
         <v>415</v>
@@ -3288,19 +3294,19 @@
         <v>38</v>
       </c>
       <c r="H37" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I37" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J37" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K37" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="L37" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M37">
         <v>1</v>
@@ -3338,19 +3344,19 @@
         <v>38</v>
       </c>
       <c r="H38" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I38" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J38" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K38" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L38" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M38">
         <v>0</v>
@@ -3388,19 +3394,19 @@
         <v>38</v>
       </c>
       <c r="H39" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I39" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J39" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K39" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L39" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M39">
         <v>0</v>
@@ -3420,10 +3426,10 @@
         <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
         <v>32</v>
@@ -3438,19 +3444,19 @@
         <v>38</v>
       </c>
       <c r="H40" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I40" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K40" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="L40" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M40">
         <v>75</v>
@@ -3470,10 +3476,10 @@
         <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D41" t="s">
         <v>32</v>
@@ -3488,19 +3494,19 @@
         <v>38</v>
       </c>
       <c r="H41" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I41" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J41" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K41" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L41" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M41">
         <v>101</v>
@@ -3520,10 +3526,10 @@
         <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D42" t="s">
         <v>32</v>
@@ -3538,19 +3544,19 @@
         <v>38</v>
       </c>
       <c r="H42" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I42" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J42" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K42" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L42" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M42">
         <v>1</v>
@@ -3570,10 +3576,10 @@
         <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D43" t="s">
         <v>32</v>
@@ -3588,19 +3594,19 @@
         <v>38</v>
       </c>
       <c r="H43" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I43" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J43" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K43" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L43" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M43">
         <v>3</v>
@@ -3620,10 +3626,10 @@
         <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -3638,19 +3644,19 @@
         <v>38</v>
       </c>
       <c r="H44" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I44" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J44" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K44" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="L44" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M44">
         <v>2</v>
@@ -3670,10 +3676,10 @@
         <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
         <v>32</v>
@@ -3688,19 +3694,19 @@
         <v>38</v>
       </c>
       <c r="H45" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I45" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J45" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K45" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="L45" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M45">
         <v>5</v>
@@ -3720,10 +3726,10 @@
         <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D46" t="s">
         <v>32</v>
@@ -3738,19 +3744,19 @@
         <v>38</v>
       </c>
       <c r="H46" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I46" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J46" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K46" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="L46" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M46">
         <v>2</v>
@@ -3770,10 +3776,10 @@
         <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
         <v>32</v>
@@ -3788,19 +3794,19 @@
         <v>38</v>
       </c>
       <c r="H47" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I47" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J47" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K47" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="L47" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M47">
         <v>2</v>
@@ -3820,10 +3826,10 @@
         <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D48" t="s">
         <v>32</v>
@@ -3838,19 +3844,19 @@
         <v>38</v>
       </c>
       <c r="H48" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I48" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J48" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K48" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L48" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M48">
         <v>1</v>
@@ -3870,10 +3876,10 @@
         <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D49" t="s">
         <v>32</v>
@@ -3888,19 +3894,19 @@
         <v>38</v>
       </c>
       <c r="H49" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I49" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J49" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K49" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="L49" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M49">
         <v>4</v>

</xml_diff>